<commit_message>
feat: menambahkan waktu alokasi dan zona waktu
</commit_message>
<xml_diff>
--- a/jadwal.xlsx
+++ b/jadwal.xlsx
@@ -5,11 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="NormalizeSchedule" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="LessonIds" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="TimeAllocation" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Timezone" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="83">
   <si>
     <t xml:space="preserve">JAM</t>
   </si>
@@ -207,6 +209,69 @@
   </si>
   <si>
     <t xml:space="preserve">SUNDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WAKTU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07.15  -  08.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08.00  -  08.45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08.45  -  09.30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09.30  -  10.15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.45  -  11.30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.30  -  12.15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.00   -  13.45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.45  -  14.30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14.30   -  15.15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15.15   -  16.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07.00  -  07.45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07.45  -  08.30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08.30  -  09.15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09.15  -  10.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.20  -  11.05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.05  -  11.50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.00  -  13.45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14.30  -  15.15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asia/Jakarta</t>
   </si>
 </sst>
 </file>
@@ -216,7 +281,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -261,6 +326,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -335,7 +407,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -388,6 +460,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,11 +483,11 @@
   </sheetPr>
   <dimension ref="A1:AG48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.09765625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.08984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="0" width="5.77"/>
@@ -5305,11 +5381,11 @@
   </sheetPr>
   <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H64" activeCellId="0" sqref="H64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.12890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.82"/>
@@ -5849,6 +5925,454 @@
       </c>
       <c r="B67" s="10" t="s">
         <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Nimbus Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Nimbus Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B48"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="8" t="n">
+        <v>5</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="8" t="n">
+        <v>8</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="8" t="n">
+        <v>9</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="8" t="n">
+        <v>5</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="8" t="n">
+        <v>8</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="8" t="n">
+        <v>9</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Nimbus Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Nimbus Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.64"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: menambahkan waktu istirahat
</commit_message>
<xml_diff>
--- a/jadwal.xlsx
+++ b/jadwal.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="88">
   <si>
     <t xml:space="preserve">JAM</t>
   </si>
@@ -226,12 +226,21 @@
     <t xml:space="preserve">09.30  -  10.15</t>
   </si>
   <si>
+    <t xml:space="preserve">isBreak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.15  -  10.45</t>
+  </si>
+  <si>
     <t xml:space="preserve">10.45  -  11.30</t>
   </si>
   <si>
     <t xml:space="preserve">11.30  -  12.15</t>
   </si>
   <si>
+    <t xml:space="preserve">12.15  -  13.00</t>
+  </si>
+  <si>
     <t xml:space="preserve">13.00   -  13.45</t>
   </si>
   <si>
@@ -256,10 +265,16 @@
     <t xml:space="preserve">09.15  -  10.00</t>
   </si>
   <si>
+    <t xml:space="preserve">10.00  -  10.20</t>
+  </si>
+  <si>
     <t xml:space="preserve">10.20  -  11.05</t>
   </si>
   <si>
     <t xml:space="preserve">11.05  -  11.50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.50  -  13.00 </t>
   </si>
   <si>
     <t xml:space="preserve">13.00  -  13.45</t>
@@ -487,7 +502,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.08984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.07421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="0" width="5.77"/>
@@ -5385,7 +5400,7 @@
       <selection pane="topLeft" activeCell="H64" activeCellId="0" sqref="H64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.12890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.11328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.82"/>
@@ -5943,15 +5958,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A50" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A58" activeCellId="0" sqref="A58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.09"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5995,347 +6010,427 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
-        <v>5</v>
+      <c r="A6" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="n">
-        <v>8</v>
+      <c r="A9" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B16" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="13" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B19" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="13" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="n">
-        <v>9</v>
+      <c r="A29" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="B30" s="13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="B32" s="13" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="8" t="n">
-        <v>3</v>
-      </c>
-      <c r="B33" s="13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="8" t="n">
-        <v>4</v>
-      </c>
-      <c r="B34" s="13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="8" t="n">
-        <v>5</v>
-      </c>
-      <c r="B35" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="8" t="n">
-        <v>6</v>
-      </c>
       <c r="B36" s="13" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="8" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="8" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="8" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="8" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="8" t="n">
-        <v>2</v>
+      <c r="A41" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="8" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="8" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="8" t="n">
-        <v>5</v>
+      <c r="A44" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="8" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="8" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="8" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="B51" s="13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B52" s="13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="8" t="n">
+        <v>5</v>
+      </c>
+      <c r="B53" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="B54" s="13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B55" s="13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="8" t="n">
+        <v>8</v>
+      </c>
+      <c r="B57" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="8" t="n">
         <v>9</v>
       </c>
-      <c r="B48" s="13" t="s">
-        <v>80</v>
+      <c r="B58" s="13" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -6360,19 +6455,19 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.64"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>